<commit_message>
♻️ Updated BaseTest, Listeners, Utilities & testng.xml | Ignored build files
</commit_message>
<xml_diff>
--- a/practice_POM_Framework/src/test/resources/test-environment.xlsx
+++ b/practice_POM_Framework/src/test/resources/test-environment.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10727"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saicharanmallampalli/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/scmallampalli/Documents/Selenium-Framework/Selenium_POM_Framework/practice_POM_Framework/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C7A280-38B1-6C43-9DCE-2A1B6DC9B2FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6F50B6-15B8-F240-AC8C-2A64EBC8E50F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16360" xr2:uid="{ED0FA195-C863-6149-8506-AFE17CBF67C7}"/>
+    <workbookView xWindow="340" yWindow="500" windowWidth="28100" windowHeight="16320" xr2:uid="{ED0FA195-C863-6149-8506-AFE17CBF67C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>